<commit_message>
Assembly instructions Figures 8-9
</commit_message>
<xml_diff>
--- a/Calibration/Load cell calibration/Load cell calibration.xlsx
+++ b/Calibration/Load cell calibration/Load cell calibration.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferrerx\Desktop\Sport analyzer\Sport Analyzer\Calibration\Load cell calibration\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferrerx\Documents\GitHub\Sport_Analyzer\Calibration\Load cell calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8663" windowHeight="3668"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8660" windowHeight="3670"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental data Horizontal" sheetId="2" r:id="rId1"/>
-    <sheet name="Experimental data Vertical" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Force (N)</t>
   </si>
@@ -597,537 +596,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Load</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> cell calibration equation</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="lineMarker"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:trendline>
-            <c:spPr>
-              <a:ln w="19050" cap="rnd">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-                <a:prstDash val="sysDot"/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:trendlineType val="linear"/>
-            <c:dispRSqr val="1"/>
-            <c:dispEq val="1"/>
-            <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="4.0191392005202886E-2"/>
-                  <c:y val="0.26352673492605233"/>
-                </c:manualLayout>
-              </c:layout>
-              <c:numFmt formatCode="General" sourceLinked="0"/>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="65000"/>
-                          <a:lumOff val="35000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
-                </a:p>
-              </c:txPr>
-            </c:trendlineLbl>
-          </c:trendline>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Experimental data Vertical'!$G$6:$G$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>7200</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>75700</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>110900</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>145400</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>180200</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>215300</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>250200</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>284800</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Experimental data Vertical'!$F$6:$F$13</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="8"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>78.48</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>117.72</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>156.96</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>196.20000000000002</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>235.44</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>274.68</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>313.92</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-14A9-44A2-9FAF-3332487957D5}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:axId val="492448488"/>
-        <c:axId val="492448160"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="492448488"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Load cell reading</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="492448160"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:valAx>
-        <c:axId val="492448160"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Force (N)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="492448488"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1683,522 +1152,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -2217,43 +1170,6 @@
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>107950</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>136525</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2539,16 +1455,16 @@
   <dimension ref="E2:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="2" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
         <v>4</v>
       </c>
@@ -2556,7 +1472,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
         <v>1</v>
       </c>
@@ -2564,7 +1480,7 @@
         <v>9.81</v>
       </c>
     </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2575,7 +1491,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E6">
         <v>0</v>
       </c>
@@ -2587,7 +1503,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E7">
         <v>8</v>
       </c>
@@ -2599,7 +1515,7 @@
         <v>75700</v>
       </c>
     </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E8">
         <v>12</v>
       </c>
@@ -2611,7 +1527,7 @@
         <v>110900</v>
       </c>
     </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E9">
         <v>16</v>
       </c>
@@ -2623,7 +1539,7 @@
         <v>145400</v>
       </c>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E10">
         <v>20</v>
       </c>
@@ -2635,7 +1551,7 @@
         <v>180200</v>
       </c>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E11">
         <v>24</v>
       </c>
@@ -2647,7 +1563,7 @@
         <v>215300</v>
       </c>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E12">
         <v>28</v>
       </c>
@@ -2659,7 +1575,7 @@
         <v>250200</v>
       </c>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.35">
       <c r="E13">
         <v>32</v>
       </c>
@@ -2676,139 +1592,4 @@
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="E3:G13"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>9.81</v>
-      </c>
-    </row>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E5" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f>E6*$F$3</f>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>7200</v>
-      </c>
-    </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7">
-        <f>E7*$F$3</f>
-        <v>78.48</v>
-      </c>
-      <c r="G7">
-        <v>75700</v>
-      </c>
-    </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E8">
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <f t="shared" ref="F8:F13" si="0">E8*$F$3</f>
-        <v>117.72</v>
-      </c>
-      <c r="G8">
-        <v>110900</v>
-      </c>
-    </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E9">
-        <v>16</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="0"/>
-        <v>156.96</v>
-      </c>
-      <c r="G9">
-        <v>145400</v>
-      </c>
-    </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E10">
-        <v>20</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="0"/>
-        <v>196.20000000000002</v>
-      </c>
-      <c r="G10">
-        <v>180200</v>
-      </c>
-    </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E11">
-        <v>24</v>
-      </c>
-      <c r="F11">
-        <f t="shared" si="0"/>
-        <v>235.44</v>
-      </c>
-      <c r="G11">
-        <v>215300</v>
-      </c>
-    </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E12">
-        <v>28</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="0"/>
-        <v>274.68</v>
-      </c>
-      <c r="G12">
-        <v>250200</v>
-      </c>
-    </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.45">
-      <c r="E13">
-        <v>32</v>
-      </c>
-      <c r="F13">
-        <f t="shared" si="0"/>
-        <v>313.92</v>
-      </c>
-      <c r="G13">
-        <v>284800</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>